<commit_message>
Uploading some more (uncomplete) experiment results
</commit_message>
<xml_diff>
--- a/madetools/core/experiment_result/experiment_Evostar2016_ALL_20151018020506.118.xlsx
+++ b/madetools/core/experiment_result/experiment_Evostar2016_ALL_20151018020506.118.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="55">
   <si>
     <t>Iteration</t>
   </si>
@@ -175,6 +175,12 @@
   </si>
   <si>
     <t>[16, 6, 8, 13, 107, 0.22794494, 0.4452618, 0.49502742, 0.49671987, 0.8618915, 0.3434298, 0.8252133, 0.35188872, 0.253882, 0.60334337, 0.10772461, 0.9619268, 0.63432795, 0.7341202, 0.62571263, 0.056640603, 0.38198394, 0.72287714, 0.5733722, 0.58295155, 0.8311927, 0.4372215, 0.63450253, 0.64060366, 0.4180851, 0.48156846, 0.5717145, 0.31652343, 0.5988041, 0.7829326, 0.46030802, 0.84714925, 0.8934676, 0.47220972, 0.29658562, 0.4961989, 0.7382493, 0.46752042, 0.7964498, 0.69236946, 0.13100669, 0.65007925, 0.5728248, 0.8340814, 0.18907633, 0.4063948, 0.78718936]</t>
+  </si>
+  <si>
+    <t>[15, 16, 9, 10, 109, 0.67601085, 0.513422, 0.2635864, 0.21835516, 0.268843, 0.41236666, 0.65258217, 0.6229082, 0.29250848, 0.528681, 0.75332034, 0.8282525, 0.5150838, 0.9204639, 0.80069244, 0.12044735, 0.2903722, 0.71965295, 0.22852382, 0.7829796, 0.30210385, 0.5443946, 0.58138466, 0.5813501, 0.34919834, 0.20638384, 0.5830844, 0.50312436, 0.54213613, 0.50839067, 0.7508806, 0.41311, 0.71007115, 0.40801752, 0.80320704, 0.9690926, 0.77518743, 0.56275654, 0.4808577, 0.80989414, 0.049788415, 0.4248149, 0.2715052, 0.13420284, 0.27404973, 0.79519796, 0.9279251]</t>
+  </si>
+  <si>
+    <t>[10, 8, 13, 7, 125, 0.56386465, 0.4863702, 0.61907876, 0.61731106, 0.5255747, 0.66833234, 0.5591835, 0.49343428, 0.50020045, 0.36494184, 0.45790708, 0.8200666, 0.81914735, 0.7505008, 0.7158586, 0.014160433, 0.2507621, 0.6299417, 0.43736744, 0.8989186, 0.29443944, 0.9440727, 0.09307182, 0.1940778, 0.3310041, 0.35835853, 0.92452115, 0.33856618, 0.4840274, 0.55174744, 0.41118985, 0.6761216, 0.9114944, 0.5781735, 0.35986722, 0.80815345, 0.6171422, 0.95544565, 0.0035003424, 0.84136665, 0.040762722, 0.57797354, 0.5832304, 0.4854872, 0.06584303, 0.29277968, 0.8486911]</t>
   </si>
 </sst>
 </file>
@@ -1588,6 +1594,282 @@
         <v>9.990858</v>
       </c>
     </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="B9" t="n">
+        <v>815.86664</v>
+      </c>
+      <c r="C9" t="n">
+        <v>278.2489</v>
+      </c>
+      <c r="D9" t="n">
+        <v>170.79956</v>
+      </c>
+      <c r="E9" t="n">
+        <v>815.86664</v>
+      </c>
+      <c r="F9" t="n">
+        <v>130.44612</v>
+      </c>
+      <c r="G9" t="n">
+        <v>30.0</v>
+      </c>
+      <c r="H9" t="s">
+        <v>53</v>
+      </c>
+      <c r="I9" t="n">
+        <v>94.26667</v>
+      </c>
+      <c r="J9" t="n">
+        <v>32.628456</v>
+      </c>
+      <c r="K9" t="n">
+        <v>418.66666</v>
+      </c>
+      <c r="L9" t="n">
+        <v>21.745129</v>
+      </c>
+      <c r="M9" t="n">
+        <v>163.93333</v>
+      </c>
+      <c r="N9" t="n">
+        <v>60.595284</v>
+      </c>
+      <c r="O9" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="P9" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Q9" t="n">
+        <v>32.033333</v>
+      </c>
+      <c r="R9" t="n">
+        <v>7.5907536</v>
+      </c>
+      <c r="S9" t="n">
+        <v>32.033333</v>
+      </c>
+      <c r="T9" t="n">
+        <v>7.5907536</v>
+      </c>
+      <c r="U9" t="n">
+        <v>13.7</v>
+      </c>
+      <c r="V9" t="n">
+        <v>6.6027684</v>
+      </c>
+      <c r="W9" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="X9" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Y9" t="n">
+        <v>32.033333</v>
+      </c>
+      <c r="Z9" t="n">
+        <v>7.5907536</v>
+      </c>
+      <c r="AA9" t="n">
+        <v>0.33333334</v>
+      </c>
+      <c r="AB9" t="n">
+        <v>1.2954384</v>
+      </c>
+      <c r="AC9" t="n">
+        <v>28.866667</v>
+      </c>
+      <c r="AD9" t="n">
+        <v>27.660172</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="B10" t="n">
+        <v>920.86664</v>
+      </c>
+      <c r="C10" t="n">
+        <v>323.1889</v>
+      </c>
+      <c r="D10" t="n">
+        <v>193.27455</v>
+      </c>
+      <c r="E10" t="n">
+        <v>920.86664</v>
+      </c>
+      <c r="F10" t="n">
+        <v>136.95172</v>
+      </c>
+      <c r="G10" t="n">
+        <v>30.0</v>
+      </c>
+      <c r="H10" t="s">
+        <v>54</v>
+      </c>
+      <c r="I10" t="n">
+        <v>41.766666</v>
+      </c>
+      <c r="J10" t="n">
+        <v>20.5723</v>
+      </c>
+      <c r="K10" t="n">
+        <v>407.96667</v>
+      </c>
+      <c r="L10" t="n">
+        <v>30.68582</v>
+      </c>
+      <c r="M10" t="n">
+        <v>240.06667</v>
+      </c>
+      <c r="N10" t="n">
+        <v>74.35606</v>
+      </c>
+      <c r="O10" t="n">
+        <v>0.033333335</v>
+      </c>
+      <c r="P10" t="n">
+        <v>0.18257418</v>
+      </c>
+      <c r="Q10" t="n">
+        <v>43.166668</v>
+      </c>
+      <c r="R10" t="n">
+        <v>7.926748</v>
+      </c>
+      <c r="S10" t="n">
+        <v>43.166668</v>
+      </c>
+      <c r="T10" t="n">
+        <v>7.926748</v>
+      </c>
+      <c r="U10" t="n">
+        <v>46.4</v>
+      </c>
+      <c r="V10" t="n">
+        <v>18.225788</v>
+      </c>
+      <c r="W10" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="X10" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Y10" t="n">
+        <v>43.166668</v>
+      </c>
+      <c r="Z10" t="n">
+        <v>7.926748</v>
+      </c>
+      <c r="AA10" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="AB10" t="n">
+        <v>0.83666</v>
+      </c>
+      <c r="AC10" t="n">
+        <v>54.833332</v>
+      </c>
+      <c r="AD10" t="n">
+        <v>23.64549</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>8.0</v>
+      </c>
+      <c r="B11" t="n">
+        <v>920.86664</v>
+      </c>
+      <c r="C11" t="n">
+        <v>369.25333</v>
+      </c>
+      <c r="D11" t="n">
+        <v>149.78954</v>
+      </c>
+      <c r="E11" t="n">
+        <v>920.86664</v>
+      </c>
+      <c r="F11" t="n">
+        <v>136.95172</v>
+      </c>
+      <c r="G11" t="n">
+        <v>30.0</v>
+      </c>
+      <c r="H11" t="s">
+        <v>54</v>
+      </c>
+      <c r="I11" t="n">
+        <v>41.766666</v>
+      </c>
+      <c r="J11" t="n">
+        <v>20.5723</v>
+      </c>
+      <c r="K11" t="n">
+        <v>407.96667</v>
+      </c>
+      <c r="L11" t="n">
+        <v>30.68582</v>
+      </c>
+      <c r="M11" t="n">
+        <v>240.06667</v>
+      </c>
+      <c r="N11" t="n">
+        <v>74.35606</v>
+      </c>
+      <c r="O11" t="n">
+        <v>0.033333335</v>
+      </c>
+      <c r="P11" t="n">
+        <v>0.18257418</v>
+      </c>
+      <c r="Q11" t="n">
+        <v>43.166668</v>
+      </c>
+      <c r="R11" t="n">
+        <v>7.926748</v>
+      </c>
+      <c r="S11" t="n">
+        <v>43.166668</v>
+      </c>
+      <c r="T11" t="n">
+        <v>7.926748</v>
+      </c>
+      <c r="U11" t="n">
+        <v>46.4</v>
+      </c>
+      <c r="V11" t="n">
+        <v>18.225788</v>
+      </c>
+      <c r="W11" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="X11" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Y11" t="n">
+        <v>43.166668</v>
+      </c>
+      <c r="Z11" t="n">
+        <v>7.926748</v>
+      </c>
+      <c r="AA11" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="AB11" t="n">
+        <v>0.83666</v>
+      </c>
+      <c r="AC11" t="n">
+        <v>54.833332</v>
+      </c>
+      <c r="AD11" t="n">
+        <v>23.64549</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="30">
     <mergeCell ref="BG1:BH1"/>
@@ -1716,6 +1998,39 @@
         <v>213.81334</v>
       </c>
     </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="B8" t="n">
+        <v>815.86664</v>
+      </c>
+      <c r="C8" t="n">
+        <v>278.2489</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="B9" t="n">
+        <v>920.86664</v>
+      </c>
+      <c r="C9" t="n">
+        <v>323.1889</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>8.0</v>
+      </c>
+      <c r="B10" t="n">
+        <v>920.86664</v>
+      </c>
+      <c r="C10" t="n">
+        <v>369.25333</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Uploading some more (uncomplete) experiment results (ALL and SHAPESHIFTER)
</commit_message>
<xml_diff>
--- a/madetools/core/experiment_result/experiment_Evostar2016_ALL_20151018020506.118.xlsx
+++ b/madetools/core/experiment_result/experiment_Evostar2016_ALL_20151018020506.118.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="56">
   <si>
     <t>Iteration</t>
   </si>
@@ -181,6 +181,9 @@
   </si>
   <si>
     <t>[10, 8, 13, 7, 125, 0.56386465, 0.4863702, 0.61907876, 0.61731106, 0.5255747, 0.66833234, 0.5591835, 0.49343428, 0.50020045, 0.36494184, 0.45790708, 0.8200666, 0.81914735, 0.7505008, 0.7158586, 0.014160433, 0.2507621, 0.6299417, 0.43736744, 0.8989186, 0.29443944, 0.9440727, 0.09307182, 0.1940778, 0.3310041, 0.35835853, 0.92452115, 0.33856618, 0.4840274, 0.55174744, 0.41118985, 0.6761216, 0.9114944, 0.5781735, 0.35986722, 0.80815345, 0.6171422, 0.95544565, 0.0035003424, 0.84136665, 0.040762722, 0.57797354, 0.5832304, 0.4854872, 0.06584303, 0.29277968, 0.8486911]</t>
+  </si>
+  <si>
+    <t>[10, 7, 11, 16, 128, 0.7680441, 0.4905956, 0.58614576, 0.6788291, 0.3286342, 0.45604947, 0.63224334, 0.58431226, 0.06409139, 0.4486112, 0.5923541, 0.86245406, 0.5781349, 0.7811539, 0.7021895, 0.0062287697, 0.40543425, 0.5332268, 0.9989835, 0.724732, 0.18392125, 0.89512044, 0.83834064, 0.31168103, 0.41456914, 0.35160974, 0.3846827, 0.40361124, 0.51614547, 0.6810796, 0.45001304, 0.36917803, 0.6831876, 0.70975894, 0.467517, 0.7663588, 0.6001911, 0.56685805, 0.74872684, 0.76030254, 0.15015125, 0.5063697, 0.17825802, 0.45337522, 0.020946769, 0.41181844, 0.53246135]</t>
   </si>
 </sst>
 </file>
@@ -1870,6 +1873,190 @@
         <v>23.64549</v>
       </c>
     </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>9.0</v>
+      </c>
+      <c r="B12" t="n">
+        <v>1109.9333</v>
+      </c>
+      <c r="C12" t="n">
+        <v>334.3911</v>
+      </c>
+      <c r="D12" t="n">
+        <v>235.51036</v>
+      </c>
+      <c r="E12" t="n">
+        <v>1109.9333</v>
+      </c>
+      <c r="F12" t="n">
+        <v>158.4918</v>
+      </c>
+      <c r="G12" t="n">
+        <v>30.0</v>
+      </c>
+      <c r="H12" t="s">
+        <v>55</v>
+      </c>
+      <c r="I12" t="n">
+        <v>37.966667</v>
+      </c>
+      <c r="J12" t="n">
+        <v>16.806164</v>
+      </c>
+      <c r="K12" t="n">
+        <v>549.86664</v>
+      </c>
+      <c r="L12" t="n">
+        <v>27.60901</v>
+      </c>
+      <c r="M12" t="n">
+        <v>291.83334</v>
+      </c>
+      <c r="N12" t="n">
+        <v>97.64647</v>
+      </c>
+      <c r="O12" t="n">
+        <v>0.033333335</v>
+      </c>
+      <c r="P12" t="n">
+        <v>0.18257418</v>
+      </c>
+      <c r="Q12" t="n">
+        <v>45.0</v>
+      </c>
+      <c r="R12" t="n">
+        <v>9.055386</v>
+      </c>
+      <c r="S12" t="n">
+        <v>45.0</v>
+      </c>
+      <c r="T12" t="n">
+        <v>9.055386</v>
+      </c>
+      <c r="U12" t="n">
+        <v>28.733334</v>
+      </c>
+      <c r="V12" t="n">
+        <v>10.599068</v>
+      </c>
+      <c r="W12" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="X12" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Y12" t="n">
+        <v>45.0</v>
+      </c>
+      <c r="Z12" t="n">
+        <v>9.055386</v>
+      </c>
+      <c r="AA12" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="AB12" t="n">
+        <v>0.48423418</v>
+      </c>
+      <c r="AC12" t="n">
+        <v>66.3</v>
+      </c>
+      <c r="AD12" t="n">
+        <v>27.327074</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="B13" t="n">
+        <v>1109.9333</v>
+      </c>
+      <c r="C13" t="n">
+        <v>518.5467</v>
+      </c>
+      <c r="D13" t="n">
+        <v>208.61398</v>
+      </c>
+      <c r="E13" t="n">
+        <v>1109.9333</v>
+      </c>
+      <c r="F13" t="n">
+        <v>158.4918</v>
+      </c>
+      <c r="G13" t="n">
+        <v>30.0</v>
+      </c>
+      <c r="H13" t="s">
+        <v>55</v>
+      </c>
+      <c r="I13" t="n">
+        <v>37.966667</v>
+      </c>
+      <c r="J13" t="n">
+        <v>16.806164</v>
+      </c>
+      <c r="K13" t="n">
+        <v>549.86664</v>
+      </c>
+      <c r="L13" t="n">
+        <v>27.60901</v>
+      </c>
+      <c r="M13" t="n">
+        <v>291.83334</v>
+      </c>
+      <c r="N13" t="n">
+        <v>97.64647</v>
+      </c>
+      <c r="O13" t="n">
+        <v>0.033333335</v>
+      </c>
+      <c r="P13" t="n">
+        <v>0.18257418</v>
+      </c>
+      <c r="Q13" t="n">
+        <v>45.0</v>
+      </c>
+      <c r="R13" t="n">
+        <v>9.055386</v>
+      </c>
+      <c r="S13" t="n">
+        <v>45.0</v>
+      </c>
+      <c r="T13" t="n">
+        <v>9.055386</v>
+      </c>
+      <c r="U13" t="n">
+        <v>28.733334</v>
+      </c>
+      <c r="V13" t="n">
+        <v>10.599068</v>
+      </c>
+      <c r="W13" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="X13" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Y13" t="n">
+        <v>45.0</v>
+      </c>
+      <c r="Z13" t="n">
+        <v>9.055386</v>
+      </c>
+      <c r="AA13" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="AB13" t="n">
+        <v>0.48423418</v>
+      </c>
+      <c r="AC13" t="n">
+        <v>66.3</v>
+      </c>
+      <c r="AD13" t="n">
+        <v>27.327074</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="30">
     <mergeCell ref="BG1:BH1"/>
@@ -2031,6 +2218,28 @@
         <v>369.25333</v>
       </c>
     </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>9.0</v>
+      </c>
+      <c r="B11" t="n">
+        <v>1109.9333</v>
+      </c>
+      <c r="C11" t="n">
+        <v>334.3911</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="B12" t="n">
+        <v>1109.9333</v>
+      </c>
+      <c r="C12" t="n">
+        <v>518.5467</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>